<commit_message>
excel summary update (sum)
</commit_message>
<xml_diff>
--- a/data/Mode_Choice_Comparison.xlsx
+++ b/data/Mode_Choice_Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhanchaoyang/Desktop/Bogota-travel-survey-comp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EBB526-1F5C-614C-87C7-7FE4574F36F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B21CF84-126F-2A48-9C4D-3F692DB70A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="35800" windowHeight="19220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="270">
   <si>
     <t>2005 MODULOD D35_MEDIO</t>
   </si>
@@ -910,6 +910,9 @@
   </si>
   <si>
     <t>feeder bus?</t>
+  </si>
+  <si>
+    <t>sum</t>
   </si>
 </sst>
 </file>
@@ -6489,7 +6492,7 @@
   <dimension ref="A1:M80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="M81" sqref="M81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -8225,7 +8228,26 @@
       <c r="M79" s="7"/>
     </row>
     <row r="80" spans="1:13" ht="19">
-      <c r="A80" s="118"/>
+      <c r="A80" s="118" t="s">
+        <v>269</v>
+      </c>
+      <c r="D80">
+        <f>SUM(D2:D73)</f>
+        <v>90617</v>
+      </c>
+      <c r="G80">
+        <f>SUM(G2:G72)</f>
+        <v>122361</v>
+      </c>
+      <c r="J80">
+        <f>SUM(J2:J73)</f>
+        <v>193459</v>
+      </c>
+      <c r="K80"/>
+      <c r="M80">
+        <f>SUM(M2:M78)</f>
+        <v>152310</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>